<commit_message>
update and insert data are now fully functional
</commit_message>
<xml_diff>
--- a/Data/NoStock.xlsx
+++ b/Data/NoStock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>BSL NO</t>
   </si>
@@ -37,190 +37,124 @@
     <t>Estimated Sales</t>
   </si>
   <si>
-    <t>Biltin</t>
-  </si>
-  <si>
-    <t>Desodin</t>
-  </si>
-  <si>
-    <t>Dinafex</t>
-  </si>
-  <si>
-    <t>Dorenta</t>
-  </si>
-  <si>
-    <t>Etorix</t>
-  </si>
-  <si>
-    <t>Fenobac</t>
-  </si>
-  <si>
-    <t>Flucloxin</t>
-  </si>
-  <si>
-    <t>Geminox</t>
-  </si>
-  <si>
-    <t>Ketonic</t>
-  </si>
-  <si>
-    <t>Kynol</t>
-  </si>
-  <si>
-    <t>Naprox</t>
-  </si>
-  <si>
-    <t>Oradin</t>
-  </si>
-  <si>
-    <t>Osticare</t>
-  </si>
-  <si>
-    <t>Rupaday</t>
-  </si>
-  <si>
-    <t>Zithrox</t>
-  </si>
-  <si>
-    <t>Biltin 20mg Tablet 30's</t>
-  </si>
-  <si>
-    <t>Desodin 60ml Syrup</t>
-  </si>
-  <si>
-    <t>Dinafex 180mg Tablet</t>
-  </si>
-  <si>
-    <t>Dinafex 60mg Tablet</t>
-  </si>
-  <si>
-    <t>Dinafex 120mg Tablet</t>
-  </si>
-  <si>
-    <t>Dorenta 50mg Tablet</t>
-  </si>
-  <si>
-    <t>Etorix 120mg Tablet</t>
-  </si>
-  <si>
-    <t>Etorix 90mg Tablet</t>
-  </si>
-  <si>
-    <t>Etorix 60mg Tablet - 40's</t>
-  </si>
-  <si>
-    <t>Fenobac 100ml Syrup</t>
-  </si>
-  <si>
-    <t>Flucloxin 500mg Capsule</t>
-  </si>
-  <si>
-    <t>Flucloxin 500mg Capsule - 36's</t>
-  </si>
-  <si>
-    <t>Geminox 320mg Tablet - 8's</t>
-  </si>
-  <si>
-    <t>Ketonic 30mg IM/IV Injection - 4's</t>
-  </si>
-  <si>
-    <t>Ketonic 30mg Injection</t>
-  </si>
-  <si>
-    <t>Ketonic 10mg Tablet</t>
-  </si>
-  <si>
-    <t>Kynol TR 100mg Capsule</t>
-  </si>
-  <si>
-    <t>Kynol TR 200mg Capsule</t>
-  </si>
-  <si>
-    <t>Kynol D 25mg Tablet</t>
-  </si>
-  <si>
-    <t>Naprox Plus 500mg Tablet - 30's</t>
-  </si>
-  <si>
-    <t>Oradin Plus Tablet - 40's</t>
-  </si>
-  <si>
-    <t>Osticare Tablet 24's</t>
-  </si>
-  <si>
-    <t>Rupaday Oral Solution 60ml</t>
-  </si>
-  <si>
-    <t>Zithrox 15ml Suspension</t>
-  </si>
-  <si>
-    <t>Zithrox 30ml Dry Suspension</t>
-  </si>
-  <si>
-    <t>Zithrox 500mg Tablet</t>
-  </si>
-  <si>
-    <t>Zithrox 250mg Tablet - 6's</t>
-  </si>
-  <si>
-    <t>30's</t>
-  </si>
-  <si>
-    <t>60 ml</t>
-  </si>
-  <si>
-    <t>50's</t>
-  </si>
-  <si>
-    <t>20's</t>
-  </si>
-  <si>
-    <t>40's</t>
-  </si>
-  <si>
-    <t>100ml</t>
-  </si>
-  <si>
-    <t>30 's</t>
-  </si>
-  <si>
-    <t>36 's</t>
-  </si>
-  <si>
-    <t>8 's</t>
-  </si>
-  <si>
-    <t>4's</t>
-  </si>
-  <si>
-    <t>5 's</t>
-  </si>
-  <si>
-    <t>50 's</t>
-  </si>
-  <si>
-    <t>60 's</t>
-  </si>
-  <si>
-    <t>40 's</t>
-  </si>
-  <si>
-    <t>24's</t>
+    <t>Alphagan</t>
+  </si>
+  <si>
+    <t>Altadin</t>
+  </si>
+  <si>
+    <t>Betagan</t>
+  </si>
+  <si>
+    <t>Bimatol</t>
+  </si>
+  <si>
+    <t>Binzotim</t>
+  </si>
+  <si>
+    <t>Combigan</t>
+  </si>
+  <si>
+    <t>Dextor OPT</t>
+  </si>
+  <si>
+    <t>Fluflam</t>
+  </si>
+  <si>
+    <t>Lotrel</t>
+  </si>
+  <si>
+    <t>Lumigan</t>
+  </si>
+  <si>
+    <t>Poly Pred</t>
+  </si>
+  <si>
+    <t>Pred OPT</t>
+  </si>
+  <si>
+    <t>Refresh Liquigel</t>
+  </si>
+  <si>
+    <t>Refresh Tears</t>
+  </si>
+  <si>
+    <t>Relestat</t>
+  </si>
+  <si>
+    <t>Zolopt</t>
+  </si>
+  <si>
+    <t>Zymar</t>
+  </si>
+  <si>
+    <t>Alphagan P 5 ml</t>
+  </si>
+  <si>
+    <t>Altadin 0.25% Ophthalmic Solution</t>
+  </si>
+  <si>
+    <t>Betagan 0.5% 5 ml</t>
+  </si>
+  <si>
+    <t>Bimatol 5ml Ophthalmic Solution</t>
+  </si>
+  <si>
+    <t>Binzotim Ophthalmic Suspension 5ml</t>
+  </si>
+  <si>
+    <t>Combigan Ophthalmic Susp 5ml</t>
+  </si>
+  <si>
+    <t>Dextor T Ophthalmic Suspension, 5ml</t>
+  </si>
+  <si>
+    <t>Fluflam 0.1% Opthalmic Suspension</t>
+  </si>
+  <si>
+    <t>Lotrel 0.5% Opthalmic Suspension</t>
+  </si>
+  <si>
+    <t>Lumigan 0.03% 3 ml</t>
+  </si>
+  <si>
+    <t>Poly Pred 5ml</t>
+  </si>
+  <si>
+    <t>PRED 5ml Ophthalmic Suspension</t>
+  </si>
+  <si>
+    <t>Refresh Liquigel 15ml</t>
+  </si>
+  <si>
+    <t>Refresh Tears 15ml</t>
+  </si>
+  <si>
+    <t>Relestat 5 ml</t>
+  </si>
+  <si>
+    <t>Zolopt Ophthalmic Suspension 5ml</t>
+  </si>
+  <si>
+    <t>Zymar 5ml</t>
+  </si>
+  <si>
+    <t>5 ml</t>
   </si>
   <si>
     <t>1's</t>
   </si>
   <si>
-    <t>15 ml</t>
-  </si>
-  <si>
-    <t>30ml</t>
-  </si>
-  <si>
-    <t>6 's</t>
-  </si>
-  <si>
-    <t>6's</t>
+    <t>5 ml.</t>
+  </si>
+  <si>
+    <t>5ml</t>
+  </si>
+  <si>
+    <t>3 ml</t>
+  </si>
+  <si>
+    <t>15ml</t>
   </si>
 </sst>
 </file>
@@ -578,7 +512,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -618,21 +552,21 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F2">
-        <v>15672</v>
+        <v>39</v>
       </c>
       <c r="G2">
-        <v>5286635</v>
+        <v>20390</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -641,10 +575,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -655,7 +589,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -664,10 +598,10 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -681,16 +615,16 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -701,19 +635,19 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -724,42 +658,42 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>54941</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -770,19 +704,19 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -793,19 +727,19 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -816,42 +750,42 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>112004</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -862,19 +796,19 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -885,19 +819,19 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -908,65 +842,65 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>2603</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>614880</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>796</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -977,254 +911,24 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19">
-        <v>12</v>
-      </c>
-      <c r="B19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19">
-        <v>18</v>
-      </c>
-      <c r="D19" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20">
-        <v>12</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20">
-        <v>19</v>
-      </c>
-      <c r="D20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21">
-        <v>17</v>
-      </c>
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21">
-        <v>20</v>
-      </c>
-      <c r="D21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22">
-        <v>19</v>
-      </c>
-      <c r="B22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22">
-        <v>21</v>
-      </c>
-      <c r="D22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23">
-        <v>20</v>
-      </c>
-      <c r="B23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23">
-        <v>22</v>
-      </c>
-      <c r="D23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24">
-        <v>23</v>
-      </c>
-      <c r="D24" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25">
-        <v>35</v>
-      </c>
-      <c r="B25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25">
-        <v>24</v>
-      </c>
-      <c r="D25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26">
-        <v>35</v>
-      </c>
-      <c r="B26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26">
-        <v>25</v>
-      </c>
-      <c r="D26" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27">
-        <v>35</v>
-      </c>
-      <c r="B27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27">
-        <v>26</v>
-      </c>
-      <c r="D27" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28">
-        <v>35</v>
-      </c>
-      <c r="B28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28">
-        <v>27</v>
-      </c>
-      <c r="D28" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
         <v>0</v>
       </c>
     </row>

</xml_diff>